<commit_message>
update: missing sessions from classes 1,2,3
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM1/project-planning/week6/WBS Estimacion de tiempo y recursos.xlsx
+++ b/PM1/project-planning/week6/WBS Estimacion de tiempo y recursos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM1\project-planning\week6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2573C1B5-D53C-4708-97EF-ADB04D895E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C89FFD57-615C-4DE8-A8A8-8AA779E7F67B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1823,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H93" sqref="H93"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4216,14 +4216,14 @@
         <v>301</v>
       </c>
       <c r="C99" s="48">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="D99" s="2">
         <v>6</v>
       </c>
       <c r="E99" s="50">
         <f>C99*D99</f>
-        <v>72000</v>
+        <v>54000</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -4233,14 +4233,14 @@
         <v>302</v>
       </c>
       <c r="C100" s="48">
-        <v>15000</v>
+        <v>14000</v>
       </c>
       <c r="D100" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E100" s="50">
         <f t="shared" ref="E100:E103" si="17">C100*D100</f>
-        <v>90000</v>
+        <v>70000</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -4250,14 +4250,14 @@
         <v>303</v>
       </c>
       <c r="C101" s="48">
-        <v>15000</v>
+        <v>14000</v>
       </c>
       <c r="D101" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E101" s="50">
         <f t="shared" si="17"/>
-        <v>90000</v>
+        <v>70000</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -4270,11 +4270,11 @@
         <v>16000</v>
       </c>
       <c r="D102" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E102" s="50">
         <f t="shared" si="17"/>
-        <v>48000</v>
+        <v>32000</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -4284,14 +4284,14 @@
         <v>305</v>
       </c>
       <c r="C103" s="56">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="D103" s="57">
         <v>8</v>
       </c>
       <c r="E103" s="58">
         <f t="shared" si="17"/>
-        <v>96000</v>
+        <v>72000</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -4304,7 +4304,7 @@
       </c>
       <c r="E104" s="50">
         <f>SUM(E98:E103)</f>
-        <v>492000</v>
+        <v>394000</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -4317,7 +4317,7 @@
       <c r="D105" s="61"/>
       <c r="E105" s="62">
         <f>E96+E104</f>
-        <v>505820</v>
+        <v>407820</v>
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>

</xml_diff>